<commit_message>
Page Admin + Chck les clients + update sprint
</commit_message>
<xml_diff>
--- a/semain 3/Feuille_de_temps_S1-Eq1.xlsx
+++ b/semain 3/Feuille_de_temps_S1-Eq1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\CoolKidsClub-Gym\semain 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4479588-B1B4-458E-9E35-DEFD02A963A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F7D402-13A3-4895-BB58-3A5BDF812D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="76">
   <si>
     <t>Temps</t>
   </si>
@@ -261,10 +261,13 @@
     <t>Regarder video pour sms</t>
   </si>
   <si>
-    <t>xH</t>
+    <t>Admin Page</t>
   </si>
   <si>
-    <t>x</t>
+    <t>Adminn Income: Essayer</t>
+  </si>
+  <si>
+    <t>Admin Clients Insert: Bug + essaye fix</t>
   </si>
 </sst>
 </file>
@@ -725,8 +728,8 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -827,7 +830,7 @@
         <v>60</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
@@ -899,8 +902,8 @@
       <c r="H11" s="7">
         <v>7</v>
       </c>
-      <c r="I11" s="7" t="s">
-        <v>74</v>
+      <c r="I11" s="7">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
@@ -1064,8 +1067,8 @@
   </sheetPr>
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1240,6 +1243,12 @@
       <c r="N4" t="s">
         <v>69</v>
       </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
@@ -1262,6 +1271,12 @@
       <c r="N5" t="s">
         <v>72</v>
       </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G6">
@@ -1275,6 +1290,12 @@
       </c>
       <c r="J6" t="s">
         <v>56</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>